<commit_message>
v4: testing and presentation update
</commit_message>
<xml_diff>
--- a/v4/Testing_v4.xlsx
+++ b/v4/Testing_v4.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\fs02.opaltelecom.com\IRLOfflineFiles$\eric.diep\Documents\GitHub\Team-Infinite\v4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.bulley\Team-Infinite\v4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -957,45 +957,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1031,15 +992,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1"/>
@@ -1050,6 +1002,54 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="3" builtinId="53"/>
@@ -1057,187 +1057,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -1616,68 +1436,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D46" zoomScale="99" workbookViewId="0">
-      <selection activeCell="R74" sqref="R74"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="S1" sqref="A1:S76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="84.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="25.54296875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" customWidth="1"/>
-    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" customWidth="1"/>
+    <col min="15" max="15" width="18.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="43" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
-      <c r="N3" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="O3" s="47" t="s">
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="78"/>
+      <c r="H3" s="78"/>
+      <c r="I3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="79"/>
+      <c r="N3" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="39" t="s">
+      <c r="P3" s="66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="42"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="46"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="69"/>
+      <c r="B4" s="71"/>
+      <c r="C4" s="73"/>
       <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
@@ -1708,11 +1528,11 @@
       <c r="M4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="48"/>
-      <c r="O4" s="48"/>
-      <c r="P4" s="40"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="67"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>1.1000000000000001</v>
       </c>
@@ -1761,7 +1581,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="16"/>
@@ -1804,7 +1624,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
@@ -1847,7 +1667,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
@@ -1890,7 +1710,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14">
         <v>1.2</v>
       </c>
@@ -1939,7 +1759,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="14"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1982,7 +1802,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="14"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2025,7 +1845,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="14"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2068,7 +1888,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2111,7 +1931,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2154,7 +1974,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="19"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -2197,7 +2017,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7">
         <v>1.3</v>
       </c>
@@ -2246,7 +2066,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="14"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2289,7 +2109,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="14"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2332,7 +2152,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2375,7 +2195,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2418,7 +2238,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="14"/>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -2461,7 +2281,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="14"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -2504,7 +2324,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="14"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2547,7 +2367,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="16" t="s">
         <v>32</v>
@@ -2592,7 +2412,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2635,7 +2455,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="14"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2678,7 +2498,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="14"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -2721,7 +2541,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="14"/>
       <c r="B28" s="16"/>
       <c r="C28" s="16"/>
@@ -2764,7 +2584,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="14"/>
       <c r="B29" s="16"/>
       <c r="C29" s="16"/>
@@ -2807,7 +2627,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="14"/>
       <c r="B30" s="16"/>
       <c r="C30" s="16"/>
@@ -2850,7 +2670,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="19"/>
       <c r="B31" s="21"/>
       <c r="C31" s="21"/>
@@ -2893,7 +2713,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A32" s="14">
         <v>1.4</v>
       </c>
@@ -2942,7 +2762,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33" s="14"/>
       <c r="B33" s="16"/>
       <c r="C33" s="16" t="s">
@@ -2987,19 +2807,19 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A37" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B37" s="43" t="s">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A37" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="72" t="s">
         <v>3</v>
       </c>
       <c r="D37" s="35" t="s">
@@ -3014,20 +2834,20 @@
       <c r="K37" s="36"/>
       <c r="L37" s="36"/>
       <c r="M37" s="37"/>
-      <c r="N37" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="O37" s="47" t="s">
+      <c r="N37" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="O37" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="P37" s="39" t="s">
+      <c r="P37" s="66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="46"/>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A38" s="69"/>
+      <c r="B38" s="71"/>
+      <c r="C38" s="73"/>
       <c r="D38" s="4" t="s">
         <v>8</v>
       </c>
@@ -3058,11 +2878,11 @@
       <c r="M38" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N38" s="48"/>
-      <c r="O38" s="48"/>
-      <c r="P38" s="40"/>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N38" s="65"/>
+      <c r="O38" s="65"/>
+      <c r="P38" s="67"/>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39" s="14">
         <v>2.1</v>
       </c>
@@ -3111,7 +2931,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -3145,19 +2965,19 @@
       <c r="M40" s="18">
         <v>5</v>
       </c>
-      <c r="N40" s="54" t="s">
+      <c r="N40" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="O40" s="54"/>
+      <c r="O40" s="41"/>
       <c r="P40" s="13" t="str">
         <f t="shared" ref="P40:P41" si="1">IF(O40=N40,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="55"/>
-      <c r="B41" s="56"/>
-      <c r="C41" s="57"/>
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A41" s="42"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="44"/>
       <c r="D41" s="32">
         <v>0</v>
       </c>
@@ -3188,24 +3008,24 @@
       <c r="M41" s="32">
         <v>0</v>
       </c>
-      <c r="N41" s="58" t="s">
+      <c r="N41" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="O41" s="58"/>
-      <c r="P41" s="64" t="str">
+      <c r="O41" s="45"/>
+      <c r="P41" s="51" t="str">
         <f t="shared" si="1"/>
         <v>FAIL</v>
       </c>
-      <c r="Q41" s="52"/>
-    </row>
-    <row r="42" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="61">
+      <c r="Q41" s="39"/>
+    </row>
+    <row r="42" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="48">
         <v>2.2000000000000002</v>
       </c>
-      <c r="B42" s="60" t="s">
+      <c r="B42" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="C42" s="62" t="s">
+      <c r="C42" s="49" t="s">
         <v>42</v>
       </c>
       <c r="D42" s="18">
@@ -3242,12 +3062,12 @@
         <v>43</v>
       </c>
       <c r="O42" s="12"/>
-      <c r="P42" s="66" t="str">
+      <c r="P42" s="53" t="str">
         <f>IF(O42=N42,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -3281,19 +3101,19 @@
       <c r="M43" s="18">
         <v>100000</v>
       </c>
-      <c r="N43" s="53" t="s">
+      <c r="N43" s="40" t="s">
         <v>55</v>
       </c>
-      <c r="O43" s="53"/>
+      <c r="O43" s="40"/>
       <c r="P43" s="38" t="str">
         <f t="shared" ref="P43:P44" si="2">IF(O43=N43,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="55"/>
-      <c r="B44" s="56"/>
-      <c r="C44" s="57" t="s">
+    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A44" s="42"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="44" t="s">
         <v>57</v>
       </c>
       <c r="D44" s="32">
@@ -3326,16 +3146,16 @@
       <c r="M44" s="32">
         <v>5</v>
       </c>
-      <c r="N44" s="58" t="s">
+      <c r="N44" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="O44" s="58"/>
-      <c r="P44" s="64" t="str">
+      <c r="O44" s="45"/>
+      <c r="P44" s="51" t="str">
         <f t="shared" si="2"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="19">
         <v>2.2999999999999998</v>
       </c>
@@ -3379,12 +3199,12 @@
         <v>46</v>
       </c>
       <c r="O45" s="24"/>
-      <c r="P45" s="65" t="str">
+      <c r="P45" s="52" t="str">
         <f t="shared" ref="P45:P48" si="3">IF(O45=N45,"PASS","FAIL")</f>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A46" s="14">
         <v>2.4</v>
       </c>
@@ -3433,11 +3253,11 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="19"/>
       <c r="B47" s="21"/>
       <c r="C47" s="21"/>
-      <c r="D47" s="59">
+      <c r="D47" s="46">
         <v>20</v>
       </c>
       <c r="E47" s="23">
@@ -3467,16 +3287,16 @@
       <c r="M47" s="23">
         <v>0</v>
       </c>
-      <c r="N47" s="58" t="s">
+      <c r="N47" s="45" t="s">
         <v>58</v>
       </c>
       <c r="O47" s="24"/>
-      <c r="P47" s="67" t="str">
+      <c r="P47" s="54" t="str">
         <f t="shared" si="3"/>
         <v>FAIL</v>
       </c>
     </row>
-    <row r="48" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A48" s="14">
         <v>2.5</v>
       </c>
@@ -3525,7 +3345,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -3533,42 +3353,42 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B53" s="43" t="s">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A53" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="45" t="s">
+      <c r="C53" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="69" t="s">
+      <c r="D53" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="E53" s="70"/>
-      <c r="F53" s="70"/>
-      <c r="G53" s="70"/>
-      <c r="H53" s="70"/>
-      <c r="I53" s="70"/>
-      <c r="J53" s="70"/>
-      <c r="K53" s="70"/>
-      <c r="L53" s="70"/>
-      <c r="M53" s="71"/>
-      <c r="N53" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="O53" s="47" t="s">
+      <c r="E53" s="75"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
+      <c r="I53" s="75"/>
+      <c r="J53" s="75"/>
+      <c r="K53" s="75"/>
+      <c r="L53" s="75"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="O53" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="P53" s="39" t="s">
+      <c r="P53" s="66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A54" s="42"/>
-      <c r="B54" s="44"/>
-      <c r="C54" s="46"/>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A54" s="69"/>
+      <c r="B54" s="71"/>
+      <c r="C54" s="73"/>
       <c r="D54" s="4" t="s">
         <v>8</v>
       </c>
@@ -3599,11 +3419,11 @@
       <c r="M54" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N54" s="48"/>
-      <c r="O54" s="48"/>
-      <c r="P54" s="40"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N54" s="65"/>
+      <c r="O54" s="65"/>
+      <c r="P54" s="67"/>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="14">
         <v>3.1</v>
       </c>
@@ -3652,8 +3472,8 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A56" s="72"/>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A56" s="56"/>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="17">
@@ -3674,30 +3494,30 @@
       <c r="I56" s="18">
         <v>15</v>
       </c>
-      <c r="J56" s="68" t="s">
+      <c r="J56" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="K56" s="68" t="s">
+      <c r="K56" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="L56" s="68" t="s">
+      <c r="L56" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="M56" s="68" t="s">
+      <c r="M56" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="N56" s="54"/>
-      <c r="O56" s="54"/>
+      <c r="N56" s="41"/>
+      <c r="O56" s="41"/>
       <c r="P56" s="13" t="str">
         <f t="shared" ref="P56:P60" si="4">IF(O56=N56,"PASS","FAIL")</f>
         <v>PASS</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="76"/>
+    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="60"/>
       <c r="B57" s="21"/>
       <c r="C57" s="21"/>
-      <c r="D57" s="77"/>
+      <c r="D57" s="61"/>
       <c r="E57" s="32"/>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
@@ -3714,10 +3534,10 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
-      <c r="B58" s="74"/>
-      <c r="C58" s="75"/>
+    <row r="58" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="57"/>
+      <c r="B58" s="58"/>
+      <c r="C58" s="59"/>
       <c r="D58" s="4" t="s">
         <v>8</v>
       </c>
@@ -3747,11 +3567,11 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="14">
         <v>3.2</v>
       </c>
-      <c r="B59" s="63"/>
+      <c r="B59" s="50"/>
       <c r="C59" s="16" t="s">
         <v>70</v>
       </c>
@@ -3761,16 +3581,16 @@
       <c r="E59" s="18">
         <v>99</v>
       </c>
-      <c r="F59" s="68" t="s">
+      <c r="F59" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="G59" s="68" t="s">
+      <c r="G59" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="H59" s="68" t="s">
+      <c r="H59" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="I59" s="68" t="s">
+      <c r="I59" s="55" t="s">
         <v>64</v>
       </c>
       <c r="J59" s="18"/>
@@ -3786,7 +3606,7 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="2"/>
       <c r="C60" s="3"/>
@@ -3796,16 +3616,16 @@
       <c r="E60" s="18">
         <v>100</v>
       </c>
-      <c r="F60" s="68" t="s">
+      <c r="F60" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="G60" s="68" t="s">
+      <c r="G60" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="H60" s="68" t="s">
+      <c r="H60" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="I60" s="68" t="s">
+      <c r="I60" s="55" t="s">
         <v>64</v>
       </c>
       <c r="J60" s="18"/>
@@ -3819,49 +3639,49 @@
         <v>PASS</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="43" t="s">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A65" s="68" t="s">
+        <v>1</v>
+      </c>
+      <c r="B65" s="70" t="s">
         <v>2</v>
       </c>
-      <c r="C65" s="45" t="s">
+      <c r="C65" s="72" t="s">
         <v>3</v>
       </c>
-      <c r="D65" s="78" t="s">
+      <c r="D65" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="E65" s="78"/>
-      <c r="F65" s="78"/>
-      <c r="G65" s="78"/>
-      <c r="H65" s="78"/>
-      <c r="I65" s="78"/>
-      <c r="J65" s="78"/>
-      <c r="K65" s="78"/>
-      <c r="L65" s="78"/>
-      <c r="M65" s="78"/>
-      <c r="N65" s="78"/>
-      <c r="O65" s="78"/>
-      <c r="P65" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q65" s="47" t="s">
+      <c r="E65" s="62"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="62"/>
+      <c r="K65" s="62"/>
+      <c r="L65" s="62"/>
+      <c r="M65" s="62"/>
+      <c r="N65" s="62"/>
+      <c r="O65" s="62"/>
+      <c r="P65" s="64" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q65" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="R65" s="39" t="s">
+      <c r="R65" s="66" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="42"/>
-      <c r="B66" s="44"/>
-      <c r="C66" s="46"/>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A66" s="69"/>
+      <c r="B66" s="71"/>
+      <c r="C66" s="73"/>
       <c r="D66" s="4" t="s">
         <v>8</v>
       </c>
@@ -3898,11 +3718,11 @@
       <c r="O66" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="P66" s="48"/>
-      <c r="Q66" s="48"/>
-      <c r="R66" s="40"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="P66" s="65"/>
+      <c r="Q66" s="65"/>
+      <c r="R66" s="67"/>
+    </row>
+    <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A67" s="14">
         <v>4.0999999999999996</v>
       </c>
@@ -3957,10 +3777,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A68" s="14"/>
       <c r="B68" s="16"/>
-      <c r="C68" s="79"/>
+      <c r="C68" s="63"/>
       <c r="D68" s="17">
         <v>20</v>
       </c>
@@ -4006,10 +3826,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A69" s="14"/>
       <c r="B69" s="16"/>
-      <c r="C69" s="79"/>
+      <c r="C69" s="63"/>
       <c r="D69" s="17">
         <v>20</v>
       </c>
@@ -4055,10 +3875,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A70" s="14"/>
       <c r="B70" s="16"/>
-      <c r="C70" s="79"/>
+      <c r="C70" s="63"/>
       <c r="D70" s="17">
         <v>20</v>
       </c>
@@ -4104,10 +3924,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A71" s="14"/>
       <c r="B71" s="16"/>
-      <c r="C71" s="79"/>
+      <c r="C71" s="63"/>
       <c r="D71" s="17">
         <v>20</v>
       </c>
@@ -4153,10 +3973,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A72" s="14"/>
       <c r="B72" s="16"/>
-      <c r="C72" s="79"/>
+      <c r="C72" s="63"/>
       <c r="D72" s="17">
         <v>20</v>
       </c>
@@ -4202,10 +4022,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A73" s="14"/>
       <c r="B73" s="16"/>
-      <c r="C73" s="79"/>
+      <c r="C73" s="63"/>
       <c r="D73" s="17">
         <v>20</v>
       </c>
@@ -4251,10 +4071,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A74" s="14"/>
       <c r="B74" s="16"/>
-      <c r="C74" s="79"/>
+      <c r="C74" s="63"/>
       <c r="D74" s="17">
         <v>20</v>
       </c>
@@ -4300,10 +4120,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A75" s="14"/>
       <c r="B75" s="16"/>
-      <c r="C75" s="79"/>
+      <c r="C75" s="63"/>
       <c r="D75" s="17">
         <v>20</v>
       </c>
@@ -4349,10 +4169,10 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A76" s="14"/>
       <c r="B76" s="16"/>
-      <c r="C76" s="79"/>
+      <c r="C76" s="63"/>
       <c r="D76" s="17">
         <v>20</v>
       </c>
@@ -4398,24 +4218,11 @@
         <v>FAIL</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
       <c r="P77" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="Q65:Q66"/>
-    <mergeCell ref="R65:R66"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="N53:N54"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="D53:M53"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
     <mergeCell ref="P3:P4"/>
     <mergeCell ref="A37:A38"/>
     <mergeCell ref="B37:B38"/>
@@ -4429,47 +4236,61 @@
     <mergeCell ref="D3:M3"/>
     <mergeCell ref="N3:N4"/>
     <mergeCell ref="O3:O4"/>
+    <mergeCell ref="N53:N54"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="D53:M53"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="Q65:Q66"/>
+    <mergeCell ref="R65:R66"/>
+    <mergeCell ref="P65:P66"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="C65:C66"/>
   </mergeCells>
   <conditionalFormatting sqref="P5:P33 P42 P45:P48">
-    <cfRule type="cellIs" dxfId="27" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="43" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="44" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="8" priority="44" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",P5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P39:P41">
-    <cfRule type="cellIs" dxfId="25" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="31" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="32" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="6" priority="32" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",P39)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P43:P44">
-    <cfRule type="cellIs" dxfId="23" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="29" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="4" priority="30" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",P43)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P55:P60">
-    <cfRule type="cellIs" dxfId="21" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="25" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="2" priority="26" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",P55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R67:R76">
-    <cfRule type="cellIs" dxfId="19" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="21" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="PASS">
+    <cfRule type="containsText" dxfId="0" priority="22" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",R67)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>